<commit_message>
work notes sync up
</commit_message>
<xml_diff>
--- a/Docs/Project/Project-Artifacts/Project-Updates/DetailedBenchmarks_readmission_Iteration1_20180509.xlsx
+++ b/Docs/Project/Project-Artifacts/Project-Updates/DetailedBenchmarks_readmission_Iteration1_20180509.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nathalieblu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Health Services Analytics\Readmissions\Docs\Project\Project-Artifacts\Project-Updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>DELIVERY</t>
   </si>
@@ -165,49 +165,6 @@
 • Plan transition toward using eConnect data for timelier predictions. 
 • Hold 3rd causal mapping session to focus on a small number of high-value diagnoses and their corresponding models This will be the end of Iteration 2. 
 </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="20"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Legend:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> In</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> orange are Qing's tasks</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. In black are Nathalie's. </t>
-    </r>
   </si>
   <si>
     <r>
@@ -258,8 +215,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,22 +282,7 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -419,7 +361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -479,86 +421,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -566,7 +428,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -623,13 +485,50 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -655,70 +554,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1003,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="50.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1015,7 +850,7 @@
     <col min="2" max="7" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -1037,207 +872,185 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="34"/>
-    </row>
-    <row r="2" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>43229</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="22" t="s">
+      <c r="B2" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="28"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="41"/>
       <c r="G2" s="8"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="37"/>
-    </row>
-    <row r="3" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>43230</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="29"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="42"/>
       <c r="G3" s="8"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="37"/>
-    </row>
-    <row r="4" spans="1:13" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>43231</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="29"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="8"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="40"/>
-    </row>
-    <row r="5" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>43234</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="47" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="21" t="s">
+      <c r="E5" s="39"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>43235</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="36"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>43236</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="49"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="39"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>43237</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="22" t="s">
+      <c r="C8" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="21"/>
-    </row>
-    <row r="9" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="39"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="25"/>
+    </row>
+    <row r="9" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>43238</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="21"/>
-    </row>
-    <row r="10" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="32"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>43241</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="50" t="s">
-        <v>37</v>
+      <c r="C10" s="31" t="s">
+        <v>36</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="29"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>43242</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="51"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="29"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>43243</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="51"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="29"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>43244</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="51"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="29"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>43245</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="52"/>
+      <c r="C14" s="33"/>
       <c r="D14" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="29"/>
+        <v>38</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="42"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>43249</v>
       </c>
@@ -1248,15 +1061,15 @@
       <c r="D15" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="29"/>
+      <c r="F15" s="42"/>
       <c r="G15" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>43250</v>
       </c>
@@ -1267,8 +1080,8 @@
       <c r="D16" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="29"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="42"/>
       <c r="G16" s="16" t="s">
         <v>9</v>
       </c>
@@ -1278,12 +1091,12 @@
         <v>43251</v>
       </c>
       <c r="B17" s="8"/>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="30"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="43"/>
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1295,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="8"/>
-      <c r="E18" s="31"/>
+      <c r="E18" s="27"/>
       <c r="F18" s="8" t="s">
         <v>1</v>
       </c>
@@ -1306,16 +1119,16 @@
         <v>43255</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="25"/>
+      <c r="F19" s="38"/>
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1323,10 +1136,10 @@
         <v>43256</v>
       </c>
       <c r="B20" s="8"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="26"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="39"/>
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1334,10 +1147,10 @@
         <v>43257</v>
       </c>
       <c r="B21" s="8"/>
-      <c r="C21" s="45"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="26"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="39"/>
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1345,10 +1158,10 @@
         <v>43258</v>
       </c>
       <c r="B22" s="8"/>
-      <c r="C22" s="45"/>
+      <c r="C22" s="23"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="26"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="39"/>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1356,10 +1169,10 @@
         <v>43259</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="45"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="26"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="39"/>
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1367,14 +1180,14 @@
         <v>43262</v>
       </c>
       <c r="B24" s="8"/>
-      <c r="C24" s="45"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="26"/>
+      <c r="F24" s="39"/>
       <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1382,10 +1195,10 @@
         <v>43263</v>
       </c>
       <c r="B25" s="8"/>
-      <c r="C25" s="45"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="26"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="39"/>
       <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1393,10 +1206,10 @@
         <v>43264</v>
       </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="46"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="26"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1408,8 +1221,8 @@
         <v>2</v>
       </c>
       <c r="D27" s="8"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="26"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1419,8 +1232,8 @@
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="26"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1430,8 +1243,8 @@
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="26"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1441,8 +1254,8 @@
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="26"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="39"/>
       <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1452,8 +1265,8 @@
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="26"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="39"/>
       <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1466,7 +1279,7 @@
       <c r="E32" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F32" s="26"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="13"/>
     </row>
     <row r="33" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1477,7 +1290,7 @@
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="27"/>
+      <c r="F33" s="40"/>
       <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1488,7 +1301,7 @@
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
-      <c r="F34" s="21" t="s">
+      <c r="F34" s="25" t="s">
         <v>11</v>
       </c>
       <c r="G34" s="8"/>
@@ -1501,7 +1314,7 @@
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="21"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1512,7 +1325,7 @@
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
-      <c r="F36" s="21"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1523,7 +1336,7 @@
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
-      <c r="F37" s="21"/>
+      <c r="F37" s="25"/>
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1540,52 +1353,45 @@
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
     </row>
     <row r="40" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
     </row>
     <row r="41" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
     </row>
     <row r="42" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="G5:G9"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="I1:M4"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C14"/>
+  <mergeCells count="19">
     <mergeCell ref="A39:G42"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D8:D9"/>
@@ -1599,6 +1405,12 @@
     <mergeCell ref="E2:E9"/>
     <mergeCell ref="F2:F17"/>
     <mergeCell ref="F19:F33"/>
+    <mergeCell ref="G5:G9"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>